<commit_message>
feat: got a ton of data
</commit_message>
<xml_diff>
--- a/data/BARMM/BASILAN.xlsx
+++ b/data/BARMM/BASILAN.xlsx
@@ -18752,7 +18752,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D391"/>
+  <dimension ref="A1:D392"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24159,347 +24159,347 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>KALANG, JINNETTE (UBJP)</t>
+          <t>KALLAHAL, GIMA (IND)</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>32</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>0.70 %</t>
+          <t>0.65 %</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>LATIP, ROGER (PDPLBN)</t>
+          <t>KALLAHAL, JHABER (PDPLBN)</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>4,233</t>
+          <t>4,809</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>99.29 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="355">
-      <c r="A355" s="1" t="inlineStr">
+          <t>98.80 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>KALLAHAL, RAJIE (IND)</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>0.53 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1" t="inlineStr">
         <is>
           <t>Over-votes</t>
         </is>
       </c>
-      <c r="B355" s="1" t="inlineStr">
+      <c r="B356" s="1" t="inlineStr">
         <is>
           <t>Under-votes</t>
         </is>
       </c>
-      <c r="C355" s="1" t="inlineStr">
+      <c r="C356" s="1" t="inlineStr">
         <is>
           <t>Valid votes</t>
         </is>
       </c>
-      <c r="D355" s="1" t="inlineStr">
+      <c r="D356" s="1" t="inlineStr">
         <is>
           <t>Votes obtained by all candidates</t>
         </is>
       </c>
     </row>
-    <row r="356">
-      <c r="A356" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="B356" t="inlineStr">
-        <is>
-          <t>1528</t>
-        </is>
-      </c>
-      <c r="C356" t="inlineStr">
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>907</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
         <is>
           <t>5817</t>
         </is>
       </c>
-      <c r="D356" t="inlineStr">
-        <is>
-          <t>4263</t>
-        </is>
-      </c>
-    </row>
-    <row r="359">
-      <c r="A359" t="inlineStr">
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>4867</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
         <is>
           <t>VICE-MAYOR</t>
         </is>
       </c>
     </row>
-    <row r="361">
-      <c r="A361" s="1" t="inlineStr">
+    <row r="362">
+      <c r="A362" s="1" t="inlineStr">
         <is>
           <t>Candidate</t>
         </is>
       </c>
-      <c r="B361" s="1" t="inlineStr">
+      <c r="B362" s="1" t="inlineStr">
         <is>
           <t>Votes</t>
         </is>
       </c>
-      <c r="C361" s="1" t="inlineStr">
+      <c r="C362" s="1" t="inlineStr">
         <is>
           <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="362">
-      <c r="A362" t="inlineStr">
-        <is>
-          <t>KALANG, JINNETTE (UBJP)</t>
-        </is>
-      </c>
-      <c r="B362" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C362" t="inlineStr">
-        <is>
-          <t>0.70 %</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
+          <t>KALANG, JINNETTE (UBJP)</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>0.70 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
           <t>LATIP, ROGER (PDPLBN)</t>
         </is>
       </c>
-      <c r="B363" t="inlineStr">
+      <c r="B364" t="inlineStr">
         <is>
           <t>4,233</t>
         </is>
       </c>
-      <c r="C363" t="inlineStr">
+      <c r="C364" t="inlineStr">
         <is>
           <t>99.29 %</t>
         </is>
       </c>
     </row>
-    <row r="365">
-      <c r="A365" s="1" t="inlineStr">
+    <row r="366">
+      <c r="A366" s="1" t="inlineStr">
         <is>
           <t>Over-votes</t>
         </is>
       </c>
-      <c r="B365" s="1" t="inlineStr">
+      <c r="B366" s="1" t="inlineStr">
         <is>
           <t>Under-votes</t>
         </is>
       </c>
-      <c r="C365" s="1" t="inlineStr">
+      <c r="C366" s="1" t="inlineStr">
         <is>
           <t>Valid votes</t>
         </is>
       </c>
-      <c r="D365" s="1" t="inlineStr">
+      <c r="D366" s="1" t="inlineStr">
         <is>
           <t>Votes obtained by all candidates</t>
         </is>
       </c>
     </row>
-    <row r="366">
-      <c r="A366" t="inlineStr">
+    <row r="367">
+      <c r="A367" t="inlineStr">
         <is>
           <t>25</t>
         </is>
       </c>
-      <c r="B366" t="inlineStr">
+      <c r="B367" t="inlineStr">
         <is>
           <t>1528</t>
         </is>
       </c>
-      <c r="C366" t="inlineStr">
+      <c r="C367" t="inlineStr">
         <is>
           <t>5817</t>
         </is>
       </c>
-      <c r="D366" t="inlineStr">
+      <c r="D367" t="inlineStr">
         <is>
           <t>4263</t>
         </is>
       </c>
     </row>
-    <row r="369">
-      <c r="A369" t="inlineStr">
+    <row r="370">
+      <c r="A370" t="inlineStr">
         <is>
           <t>MEMBER, SANGGUNIANG BAYAN</t>
         </is>
       </c>
     </row>
-    <row r="371">
-      <c r="A371" s="1" t="inlineStr">
+    <row r="372">
+      <c r="A372" s="1" t="inlineStr">
         <is>
           <t>Candidate</t>
         </is>
       </c>
-      <c r="B371" s="1" t="inlineStr">
+      <c r="B372" s="1" t="inlineStr">
         <is>
           <t>Votes</t>
         </is>
       </c>
-      <c r="C371" s="1" t="inlineStr">
+      <c r="C372" s="1" t="inlineStr">
         <is>
           <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="372">
-      <c r="A372" t="inlineStr">
-        <is>
-          <t>ABDURAHMAN, ALIH (PDPLBN)</t>
-        </is>
-      </c>
-      <c r="B372" t="inlineStr">
-        <is>
-          <t>3,369</t>
-        </is>
-      </c>
-      <c r="C372" t="inlineStr">
-        <is>
-          <t>8.96 %</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>ABDURAJAK, SAUD (LP)</t>
+          <t>ABDURAHMAN, ALIH (PDPLBN)</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>3,404</t>
+          <t>3,369</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>9.05 %</t>
+          <t>8.96 %</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>ABUBAKAR, SAIBIN (PDPLBN)</t>
+          <t>ABDURAJAK, SAUD (LP)</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>3,404</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>0.25 %</t>
+          <t>9.05 %</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>ABUBAKAR, SALIM (IND)</t>
+          <t>ABUBAKAR, SAIBIN (PDPLBN)</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>94</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>0.07 %</t>
+          <t>0.25 %</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>AMIN, AIDA (IND)</t>
+          <t>ABUBAKAR, SALIM (IND)</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>314</t>
+          <t>30</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>0.83 %</t>
+          <t>0.07 %</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>ISALIN, SALIHIN (PDPLBN)</t>
+          <t>AMIN, AIDA (IND)</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>543</t>
+          <t>314</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>1.44 %</t>
+          <t>0.83 %</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>KALANG, HUSIN (LAKAS)</t>
+          <t>ISALIN, SALIHIN (PDPLBN)</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>2,833</t>
+          <t>543</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>7.54 %</t>
+          <t>1.44 %</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>KALANG, JEMAR (PDPLBN)</t>
+          <t>KALANG, HUSIN (LAKAS)</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>2,573</t>
+          <t>2,833</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>6.84 %</t>
+          <t>7.54 %</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>KALANG, MUJIB (PDPLBN)</t>
+          <t>KALANG, JEMAR (PDPLBN)</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -24516,178 +24516,195 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>KALANG, USMAN (LP)</t>
+          <t>KALANG, MUJIB (PDPLBN)</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>3,831</t>
+          <t>2,573</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>10.19 %</t>
+          <t>6.84 %</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>KALLAHAL, ABDULSAMIE (PDPLBN)</t>
+          <t>KALANG, USMAN (LP)</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>4,468</t>
+          <t>3,831</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>11.89 %</t>
+          <t>10.19 %</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>KASIM, PING (IND)</t>
+          <t>KALLAHAL, ABDULSAMIE (PDPLBN)</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>3,259</t>
+          <t>4,468</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>8.67 %</t>
+          <t>11.89 %</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>KESENG, HAPIJA (LP)</t>
+          <t>KASIM, PING (IND)</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>3,624</t>
+          <t>3,259</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>9.64 %</t>
+          <t>8.67 %</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>NUHI, WALID (IND)</t>
+          <t>KESENG, HAPIJA (LP)</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>3,624</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>0.75 %</t>
+          <t>9.64 %</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>SAALA, BASIR (IND)</t>
+          <t>NUHI, WALID (IND)</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>284</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>0.22 %</t>
+          <t>0.75 %</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>SALAIN, UZAIR (IND)</t>
+          <t>SAALA, BASIR (IND)</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>2,800</t>
+          <t>86</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>7.45 %</t>
+          <t>0.22 %</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
+          <t>SALAIN, UZAIR (IND)</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>2,800</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>7.45 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
           <t>TARANG, HAMAD (PDPLBN)</t>
         </is>
       </c>
-      <c r="B388" t="inlineStr">
+      <c r="B389" t="inlineStr">
         <is>
           <t>3,487</t>
         </is>
       </c>
-      <c r="C388" t="inlineStr">
+      <c r="C389" t="inlineStr">
         <is>
           <t>9.28 %</t>
         </is>
       </c>
     </row>
-    <row r="390">
-      <c r="A390" s="1" t="inlineStr">
+    <row r="391">
+      <c r="A391" s="1" t="inlineStr">
         <is>
           <t>Over-votes</t>
         </is>
       </c>
-      <c r="B390" s="1" t="inlineStr">
+      <c r="B391" s="1" t="inlineStr">
         <is>
           <t>Under-votes</t>
         </is>
       </c>
-      <c r="C390" s="1" t="inlineStr">
+      <c r="C391" s="1" t="inlineStr">
         <is>
           <t>Valid votes</t>
         </is>
       </c>
-      <c r="D390" s="1" t="inlineStr">
+      <c r="D391" s="1" t="inlineStr">
         <is>
           <t>Votes obtained by all candidates</t>
         </is>
       </c>
     </row>
-    <row r="391">
-      <c r="A391" t="inlineStr">
+    <row r="392">
+      <c r="A392" t="inlineStr">
         <is>
           <t>132</t>
         </is>
       </c>
-      <c r="B391" t="inlineStr">
+      <c r="B392" t="inlineStr">
         <is>
           <t>7900</t>
         </is>
       </c>
-      <c r="C391" t="inlineStr">
+      <c r="C392" t="inlineStr">
         <is>
           <t>46536</t>
         </is>
       </c>
-      <c r="D391" t="inlineStr">
+      <c r="D392" t="inlineStr">
         <is>
           <t>37572</t>
         </is>
@@ -43155,7 +43172,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D412"/>
+  <dimension ref="A1:D410"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -48562,892 +48579,858 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>AHIRI, NORA (IND)</t>
+          <t>FURIGAY, GEM (UNA)</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>33,576</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>0.63 %</t>
+          <t>96.66 %</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>ALLIK, JUN (LAKAS)</t>
+          <t>INJANG, MICHAEL (IND)</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>1,158</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>0.18 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="354">
-      <c r="A354" t="inlineStr">
-        <is>
-          <t>FURIGAY, ORIC (PDPLBN)</t>
-        </is>
-      </c>
-      <c r="B354" t="inlineStr">
-        <is>
-          <t>35,392</t>
-        </is>
-      </c>
-      <c r="C354" t="inlineStr">
-        <is>
-          <t>92.42 %</t>
+          <t>3.33 %</t>
         </is>
       </c>
     </row>
     <row r="355">
-      <c r="A355" t="inlineStr">
-        <is>
-          <t>SAKKALAHUL, AL-RASHEED (PFP)</t>
-        </is>
-      </c>
-      <c r="B355" t="inlineStr">
-        <is>
-          <t>2,583</t>
-        </is>
-      </c>
-      <c r="C355" t="inlineStr">
-        <is>
-          <t>6.74 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="357">
-      <c r="A357" s="1" t="inlineStr">
+      <c r="A355" s="1" t="inlineStr">
         <is>
           <t>Over-votes</t>
         </is>
       </c>
-      <c r="B357" s="1" t="inlineStr">
+      <c r="B355" s="1" t="inlineStr">
         <is>
           <t>Under-votes</t>
         </is>
       </c>
-      <c r="C357" s="1" t="inlineStr">
+      <c r="C355" s="1" t="inlineStr">
         <is>
           <t>Valid votes</t>
         </is>
       </c>
-      <c r="D357" s="1" t="inlineStr">
+      <c r="D355" s="1" t="inlineStr">
         <is>
           <t>Votes obtained by all candidates</t>
         </is>
       </c>
     </row>
-    <row r="358">
-      <c r="A358" t="inlineStr">
-        <is>
-          <t>194</t>
-        </is>
-      </c>
-      <c r="B358" t="inlineStr">
-        <is>
-          <t>3129</t>
-        </is>
-      </c>
-      <c r="C358" t="inlineStr">
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>6862</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
         <is>
           <t>41679</t>
         </is>
       </c>
-      <c r="D358" t="inlineStr">
-        <is>
-          <t>38291</t>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>34734</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>VICE-MAYOR</t>
         </is>
       </c>
     </row>
     <row r="361">
-      <c r="A361" t="inlineStr">
-        <is>
-          <t>VICE-MAYOR</t>
+      <c r="A361" s="1" t="inlineStr">
+        <is>
+          <t>Candidate</t>
+        </is>
+      </c>
+      <c r="B361" s="1" t="inlineStr">
+        <is>
+          <t>Votes</t>
+        </is>
+      </c>
+      <c r="C361" s="1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>FURIGAY, GEM (UNA)</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>33,576</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>96.66 %</t>
         </is>
       </c>
     </row>
     <row r="363">
-      <c r="A363" s="1" t="inlineStr">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>INJANG, MICHAEL (IND)</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>1,158</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>3.33 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1" t="inlineStr">
+        <is>
+          <t>Over-votes</t>
+        </is>
+      </c>
+      <c r="B365" s="1" t="inlineStr">
+        <is>
+          <t>Under-votes</t>
+        </is>
+      </c>
+      <c r="C365" s="1" t="inlineStr">
+        <is>
+          <t>Valid votes</t>
+        </is>
+      </c>
+      <c r="D365" s="1" t="inlineStr">
+        <is>
+          <t>Votes obtained by all candidates</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>6862</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>41679</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>34734</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>MEMBER, SANGGUNIANG PANLUNGSOD</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="inlineStr">
         <is>
           <t>Candidate</t>
         </is>
       </c>
-      <c r="B363" s="1" t="inlineStr">
+      <c r="B371" s="1" t="inlineStr">
         <is>
           <t>Votes</t>
         </is>
       </c>
-      <c r="C363" s="1" t="inlineStr">
+      <c r="C371" s="1" t="inlineStr">
         <is>
           <t>Percentage</t>
         </is>
       </c>
     </row>
-    <row r="364">
-      <c r="A364" t="inlineStr">
-        <is>
-          <t>FURIGAY, GEM (UNA)</t>
-        </is>
-      </c>
-      <c r="B364" t="inlineStr">
-        <is>
-          <t>33,576</t>
-        </is>
-      </c>
-      <c r="C364" t="inlineStr">
-        <is>
-          <t>96.66 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="365">
-      <c r="A365" t="inlineStr">
-        <is>
-          <t>INJANG, MICHAEL (IND)</t>
-        </is>
-      </c>
-      <c r="B365" t="inlineStr">
-        <is>
-          <t>1,158</t>
-        </is>
-      </c>
-      <c r="C365" t="inlineStr">
-        <is>
-          <t>3.33 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="367">
-      <c r="A367" s="1" t="inlineStr">
-        <is>
-          <t>Over-votes</t>
-        </is>
-      </c>
-      <c r="B367" s="1" t="inlineStr">
-        <is>
-          <t>Under-votes</t>
-        </is>
-      </c>
-      <c r="C367" s="1" t="inlineStr">
-        <is>
-          <t>Valid votes</t>
-        </is>
-      </c>
-      <c r="D367" s="1" t="inlineStr">
-        <is>
-          <t>Votes obtained by all candidates</t>
-        </is>
-      </c>
-    </row>
-    <row r="368">
-      <c r="A368" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="B368" t="inlineStr">
-        <is>
-          <t>6862</t>
-        </is>
-      </c>
-      <c r="C368" t="inlineStr">
-        <is>
-          <t>41679</t>
-        </is>
-      </c>
-      <c r="D368" t="inlineStr">
-        <is>
-          <t>34734</t>
-        </is>
-      </c>
-    </row>
-    <row r="371">
-      <c r="A371" t="inlineStr">
-        <is>
-          <t>MEMBER, SANGGUNIANG PANLUNGSOD</t>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>ABBAS, RHADAMEER (PDPLBN)</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>10,773</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>3.36 %</t>
         </is>
       </c>
     </row>
     <row r="373">
-      <c r="A373" s="1" t="inlineStr">
-        <is>
-          <t>Candidate</t>
-        </is>
-      </c>
-      <c r="B373" s="1" t="inlineStr">
-        <is>
-          <t>Votes</t>
-        </is>
-      </c>
-      <c r="C373" s="1" t="inlineStr">
-        <is>
-          <t>Percentage</t>
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>ACAR, PILAR (IND)</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>521</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>0.16 %</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>ABBAS, RHADAMEER (PDPLBN)</t>
+          <t>AKBAR, IN (PDPLBN)</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>10,773</t>
+          <t>17,879</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>3.36 %</t>
+          <t>5.58 %</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>ACAR, PILAR (IND)</t>
+          <t>AKILIN, BOY (IND)</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>521</t>
+          <t>1,126</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>0.16 %</t>
+          <t>0.35 %</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>AKBAR, IN (PDPLBN)</t>
+          <t>ALKIE, ASBIE (IND)</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>17,879</t>
+          <t>12,360</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>5.58 %</t>
+          <t>3.86 %</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>AKILIN, BOY (IND)</t>
+          <t>ANTONIO, REGINE (IND)</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>1,126</t>
+          <t>19,307</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>0.35 %</t>
+          <t>6.03 %</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>ALKIE, ASBIE (IND)</t>
+          <t>ASALUL, ANDY (UBJP)</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>12,360</t>
+          <t>1,035</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>3.86 %</t>
+          <t>0.32 %</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>ANTONIO, REGINE (IND)</t>
+          <t>ASNAWIE, SUADA (IND)</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>19,307</t>
+          <t>12,687</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>6.03 %</t>
+          <t>3.96 %</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>ASALUL, ANDY (UBJP)</t>
+          <t>ATAIN, HADJI SAMAD (PDPLBN)</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>1,035</t>
+          <t>12,133</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>0.32 %</t>
+          <t>3.79 %</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>ASNAWIE, SUADA (IND)</t>
+          <t>AWALUN, TAPS (IND)</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>12,687</t>
+          <t>428</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>3.96 %</t>
+          <t>0.13 %</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>ATAIN, HADJI SAMAD (PDPLBN)</t>
+          <t>CALIMAG, RYAN (PFP)</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>12,133</t>
+          <t>1,625</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>3.79 %</t>
+          <t>0.50 %</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>AWALUN, TAPS (IND)</t>
+          <t>CAMAL, HAMID (PFP)</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>428</t>
+          <t>1,424</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>0.13 %</t>
+          <t>0.44 %</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>CALIMAG, RYAN (PFP)</t>
+          <t>CERVANTES, SAMBOY (PDPLBN)</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>1,625</t>
+          <t>22,965</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>0.50 %</t>
+          <t>7.17 %</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>CAMAL, HAMID (PFP)</t>
+          <t>CUEVAS, JAMILA (IND)</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>1,424</t>
+          <t>634</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>0.44 %</t>
+          <t>0.19 %</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>CERVANTES, SAMBOY (PDPLBN)</t>
+          <t>DALAWIS, JING (PDPLBN)</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>22,965</t>
+          <t>14,590</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>7.17 %</t>
+          <t>4.55 %</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>CUEVAS, JAMILA (IND)</t>
+          <t>DALIPE, NONOY (IND)</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>634</t>
+          <t>15,114</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>0.19 %</t>
+          <t>4.72 %</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>DALAWIS, JING (PDPLBN)</t>
+          <t>EISMA, ARLEIGH (PDPLBN)</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>14,590</t>
+          <t>25,449</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>4.55 %</t>
+          <t>7.95 %</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>DALIPE, NONOY (IND)</t>
+          <t>FLORES, JESSICA (PFP)</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>15,114</t>
+          <t>11,668</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>4.72 %</t>
+          <t>3.64 %</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>EISMA, ARLEIGH (PDPLBN)</t>
+          <t>FLORES, KENNY (PDPLBN)</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>25,449</t>
+          <t>23,523</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>7.95 %</t>
+          <t>7.35 %</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>FLORES, JESSICA (PFP)</t>
+          <t>FRANCISCO, LUCIANO (IND)</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>11,668</t>
+          <t>520</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>3.64 %</t>
+          <t>0.16 %</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>FLORES, KENNY (PDPLBN)</t>
+          <t>FURIGAY, WILFREDO JR. (PFP)</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>23,523</t>
+          <t>6,088</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>7.35 %</t>
+          <t>1.90 %</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>FRANCISCO, LUCIANO (IND)</t>
+          <t>GUNONG, ABUBAKAR (IND)</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>14,651</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>0.16 %</t>
+          <t>4.57 %</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>FURIGAY, WILFREDO JR. (PFP)</t>
+          <t>HASSAN, IBS (PDPLBN)</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>6,088</t>
+          <t>17,222</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>1.90 %</t>
+          <t>5.38 %</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>GUNONG, ABUBAKAR (IND)</t>
+          <t>JALANI, PRASAD (IND)</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>14,651</t>
+          <t>437</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>4.57 %</t>
+          <t>0.13 %</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>HASSAN, IBS (PDPLBN)</t>
+          <t>MANGKABUNG, ROMY (PFP)</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>17,222</t>
+          <t>9,802</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>5.38 %</t>
+          <t>3.06 %</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>JALANI, PRASAD (IND)</t>
+          <t>MANIGOS, CECILIA (IND)</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>437</t>
+          <t>1,053</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>0.13 %</t>
+          <t>0.32 %</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>MANGKABUNG, ROMY (PFP)</t>
+          <t>MATEO, ROY (PFP)</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>9,802</t>
+          <t>9,033</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>3.06 %</t>
+          <t>2.82 %</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>MANIGOS, CECILIA (IND)</t>
+          <t>MOCOY, JULIETA (IND)</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>1,053</t>
+          <t>475</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>0.32 %</t>
+          <t>0.14 %</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>MATEO, ROY (PFP)</t>
+          <t>NACORDA, BENNIE (IND)</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>9,033</t>
+          <t>2,567</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>2.82 %</t>
+          <t>0.80 %</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>MOCOY, JULIETA (IND)</t>
+          <t>NISAL, FAHAD (LP)</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>475</t>
+          <t>10,992</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>0.14 %</t>
+          <t>3.43 %</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>NACORDA, BENNIE (IND)</t>
+          <t>PANGLIAS, ABZHAR (BUP)</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>2,567</t>
+          <t>12,095</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>0.80 %</t>
+          <t>3.77 %</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>NISAL, FAHAD (LP)</t>
+          <t>PURI, BOY (PDPLBN)</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>10,992</t>
+          <t>12,704</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>3.43 %</t>
+          <t>3.97 %</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>PANGLIAS, ABZHAR (BUP)</t>
+          <t>RAMOS, TITO (PFP)</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>12,095</t>
+          <t>3,408</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>3.77 %</t>
+          <t>1.06 %</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>PURI, BOY (PDPLBN)</t>
+          <t>SAN JUAN, ITOY (PDPLBN)</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>12,704</t>
+          <t>11,657</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>3.97 %</t>
+          <t>3.64 %</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>RAMOS, TITO (PFP)</t>
+          <t>ULLOH, MOHAMMAD KUSIN (PFP)</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>3,408</t>
+          <t>1,382</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>1.06 %</t>
+          <t>0.43 %</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>SAN JUAN, ITOY (PDPLBN)</t>
+          <t>YUNUS, ALBIYA (IND)</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>11,657</t>
+          <t>659</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>3.64 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="408">
-      <c r="A408" t="inlineStr">
-        <is>
-          <t>ULLOH, MOHAMMAD KUSIN (PFP)</t>
-        </is>
-      </c>
-      <c r="B408" t="inlineStr">
-        <is>
-          <t>1,382</t>
-        </is>
-      </c>
-      <c r="C408" t="inlineStr">
-        <is>
-          <t>0.43 %</t>
+          <t>0.20 %</t>
         </is>
       </c>
     </row>
     <row r="409">
-      <c r="A409" t="inlineStr">
-        <is>
-          <t>YUNUS, ALBIYA (IND)</t>
-        </is>
-      </c>
-      <c r="B409" t="inlineStr">
-        <is>
-          <t>659</t>
-        </is>
-      </c>
-      <c r="C409" t="inlineStr">
-        <is>
-          <t>0.20 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="411">
-      <c r="A411" s="1" t="inlineStr">
+      <c r="A409" s="1" t="inlineStr">
         <is>
           <t>Over-votes</t>
         </is>
       </c>
-      <c r="B411" s="1" t="inlineStr">
+      <c r="B409" s="1" t="inlineStr">
         <is>
           <t>Under-votes</t>
         </is>
       </c>
-      <c r="C411" s="1" t="inlineStr">
+      <c r="C409" s="1" t="inlineStr">
         <is>
           <t>Valid votes</t>
         </is>
       </c>
-      <c r="D411" s="1" t="inlineStr">
+      <c r="D409" s="1" t="inlineStr">
         <is>
           <t>Votes obtained by all candidates</t>
         </is>
       </c>
     </row>
-    <row r="412">
-      <c r="A412" t="inlineStr">
+    <row r="410">
+      <c r="A410" t="inlineStr">
         <is>
           <t>1637</t>
         </is>
       </c>
-      <c r="B412" t="inlineStr">
+      <c r="B410" t="inlineStr">
         <is>
           <t>79784</t>
         </is>
       </c>
-      <c r="C412" t="inlineStr">
+      <c r="C410" t="inlineStr">
         <is>
           <t>416790</t>
         </is>
       </c>
-      <c r="D412" t="inlineStr">
+      <c r="D410" t="inlineStr">
         <is>
           <t>319986</t>
         </is>

</xml_diff>